<commit_message>
Still need to implement Sentiment Analysis and Error Handling
</commit_message>
<xml_diff>
--- a/CatchAll.xlsx
+++ b/CatchAll.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,32 +476,32 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>Advisors</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>automotivepower</t>
+          <t>Hella Ventures</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Global Automotive Power Management IC Market 2021 | Growth, Share, Trends, Opportunities And Focuses On Top Key Players |ROHM, Richtek, Dialog, Allegro MicroSystems – The Manomet Current</t>
+          <t>EV Relay Market Size, Industry Trends and Forecast to 2028 | Major Players – Panasonic, TE Connectivity, Omron, HELLA, Fujitsu, LSIS – The Courier</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>The Courier</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/global-automotive-power-management-ic-market-2021-growth-share-trends-opportunities-and-focuses-on-top-key-players-rohm-richtek-dialog-allegro-microsystems/</t>
+          <t>https://www.mccourier.com/ev-relay-market-size-industry-trends-and-forecast-to-2028-major-players-panasonic-te-connectivity-omron-hella-fujitsu-lsis/</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>06/10/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -516,32 +516,32 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Company</t>
+          <t>Advisors</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>automotivepower</t>
+          <t>Hella Ventures</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Global Automotive Power Module Market 2021 | Growth, Share, Trends, Opportunities And Focuses On Top Key Players |Fuji Electric Co, Rohm Semiconductor, Mitsubishi Electric Corporation, Renesas Electronics Corporation – The Manomet Current</t>
+          <t>Global Vehicle Security Market demand 2021 | Continental, Delphi Automotive, Hella KGaA Hueck, Tokai Rika – KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/global-automotive-power-module-market-2021-growth-share-trends-opportunities-and-focuses-on-top-key-players-fuji-electric-co-rohm-semiconductor-mitsubishi-electric-corporation-renesas-electro/</t>
+          <t>https://ksusentinel.com/2021/06/16/global-vehicle-security-market-demand-2021-continental-delphi-automotive-hella-kgaa-hueck-tokai-rika/</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>06/10/2021</t>
+          <t>06/15/2021</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -552,7 +552,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -566,22 +566,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Automotive Power Inverters Market Growth Insights, Sales Projection, Future Trends, COVID-19 Impact, Size Value and Share Analysis By 2028 – KSU | The Sentinel Newspaper</t>
+          <t>Key Foundry Offers ABOV Semiconductor Gen2 Flash Memory Embedded 0.13 micron BCD Process Suitable for Automotive Power Semiconductor</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>KSU | The Sentinel Newspaper</t>
+          <t>PRNewswire</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://ksusentinel.com/2021/06/11/automotive-power-inverters-market-growth-insights-sales-projection-future-trends-covid-19-impact-size-value-and-share-analysis-by-2028/</t>
+          <t>https://www.prnewswire.com/news-releases/key-foundry-offers-abov-semiconductor-gen2-flash-memory-embedded-0-13-micron-bcd-process-suitable-for-automotive-power-semiconductor-301312052.html</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>06/11/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -592,7 +592,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -606,7 +606,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Global Automotive Power Electronics In Electric Vehicles Market 2021 | Growth, Share, Trends, Opportunities And Focuses On Top Key Players |Texas Instruments, Toshiba, Vishay Intertechnology, Kongsberg automotive – The Manomet Current</t>
+          <t>Automotive Power Distribution Modules Market Size, Trends, Growth, Scope, Overall Analysis and Forecast by 2028 – The Manomet Current</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -616,15 +616,1375 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/global-automotive-power-electronics-in-electric-vehicles-market-2021-growth-share-trends-opportunities-and-focuses-on-top-key-players-texas-instruments-toshiba-vishay-intertechnology-kongsber/</t>
+          <t>https://manometcurrent.com/automotive-power-distribution-modules-market-size-trends-growth-scope-overall-analysis-and-forecast-by-2028/</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>06/10/2021</t>
+          <t>06/15/2021</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Lithium Balance</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>Lithium Balance</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Environment + Energy Leader</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>Lithium Balance Sales</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Environment + Energy Leader</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Lithium Balance Sales</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Lithium Balance Battery Management System</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Environment + Energy Leader</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Lithium Balance Battery Management System</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Sensata</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Manual Disconnect Switch Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – ABB, Sensata Technologies, Omega Engineering, Schneider Electric, Walther-Werke, TTI – The Manomet Current</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/manual-disconnect-switch-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-abb-sensata-technologies-omega-engineering-schneider-electric-walther-werke-tti/</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Sensata</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Electromechanical Pressure Switch Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – GTE Elettromeccanica, ENERPAC, Norgren, IMI Precision Engineering, Sensata Technologies, Barksdale – The Manomet Current</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/electromechanical-pressure-switch-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-gte-elettromeccanica-enerpac-norgren-imi-precision-engineering-sensata-technol/</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Sensata Battery Management System</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Automotive Pressure Sensors Market 2021: Analysis by Business Development, Concentration Rate| Infineon Technologies AG, Sensata Technologies Inc, Texas Instruments Incorporated – The Manomet Current</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/automotive-pressure-sensors-market-2021-analysis-by-business-development-concentration-rate-infineon-technologies-ag-sensata-technologies-inc-texas-instruments-incorporated/</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>06/14/2021</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Competitor</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Sensata Battery Management System</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Global Automotive MEMS Sensors Market 2021: Segmentation Application, Technology &amp; Market Analysis Research Report to 2024 – Out 'n Proud</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Out 'n Proud</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>https://onpblog.com/uncategorized/30573/global-automotive-mems-sensors-market-2021-segmentation-application-technology-market-analysis-research-report-to-2024/</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Customer</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>Lordstown</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Company with ties to Lordstown Motors to challenge USPS contract decision</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>WFMJ</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>https://www.wfmj.com/story/44116835/company-with-ties-to-lordstown-motors-to-challenge-usps-contract-decision</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Customer</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Lordstown</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Lordstown's Struggles Raise New Fears About SPACs</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>The New York Times</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>https://www.nytimes.com/2021/06/15/business/dealbook/lordstown-spacs-sec.html</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Battery Management System</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Environment + Energy Leader</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Battery Management System</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Electric Vehicle Battery Management System Market Trends 2021 Share, Growth Factor, Industry Size, Major Key Players, Type and Analysis with Covid-19 Impact till 2027 – The Manomet Current</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>The Manomet Current</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>https://manometcurrent.com/electric-vehicle-battery-management-system-market-trends-2021-share-growth-factor-industry-size-major-key-players-type-and-analysis-with-covid-19-impact-till-2027/</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Battery Management System Cloud</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>PRNewswire</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>Battery Management System Cloud</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Lincoln to introduce four new battery-electric vehicles starting next year</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>The Detroit News</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>https://www.detroitnews.com/story/business/autos/ford/2021/06/16/lincoln-introduce-four-new-battery-electric-vehicles-starting-next-year/7693304002/</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>Battery Management System BMS</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>PRNewswire</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>Battery Management System BMS</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Leclanché introduces new generation of Li-ion modules for e-transport; high-volume production line</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Green Car Congress</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>https://www.greencarcongress.com/2021/06/20210616-leclanche.html</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>CCS</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Christopher’s Fantastic Four headed to CCS Track and Field Finals</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Gilroy Dispatch</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>https://gilroydispatch.com/christophers-fantastic-four-headed-to-ccs-track-and-field-finals/</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>CCS</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>San Juan coal plant stays open for CCS conversion</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Power Engineering International</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>https://www.powerengineeringint.com/coal-fired/san-juan-coal-plant-stays-open-for-ccs-conversion/</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Electric Vehicle Charge Controller</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Delta-Q Technologies Launches the new XV3300 Battery Charging Solution</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Rental Equipment Register</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>https://www.rermag.com/directory/automotive-tools-equipment/batteries/article/21167043/deltaq-technologies-launches-the-new-xv3300-battery-charging-solution</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>Electric Vehicle Charge Controller</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Everything we know about the Huawei Seres SF5 SUV</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Illinoisnewstoday.com</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>https://illinoisnewstoday.com/everything-we-know-about-the-huawei-seres-sf5-suv/249924/</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>06/14/2021</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Electric Vehicle Charge Controller EVCC</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Electric Vehicle Communication Controllers market 2021-2028: ABB Ltd. BYD Co Ltd. ENGIE Ficosa International SA LG INNOTEK Mitsubishi Electric Corporation Robert Bosch GmbH Schneider Electric SE Siemens AG Tesla, Inc. – Miner News</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Miner News</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>https://minernews.io/space/193144/electric-vehicle-communication-controllers-market-2021-2028-abb-ltd-byd-co-ltd-engie-ficosa-international-s-a-lg-innotek-mitsubishi-electric-corporation-robert-2/</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>Fast Charge Junction Box</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>County to kick-off 250th celebration</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Mount Airy News</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>https://www.mtairynews.com/news/98435/county-to-kick-off-250th-celebration</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Fast Charge Junction Box</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Open House offers glimpse to the past</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Mount Airy News</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>https://www.mtairynews.com/news/98431/open-house-offers-glimpse-to-the-past</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>DC-DC Converter</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>High-voltage DC-DC converters for power electronics in noise-sensitive applications introduced by TDK Lambda</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Military &amp; Aerospace Electronics</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://www.militaryaerospace.com/power/article/14205250/dcdc-converters-power-highvoltage</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>DC-DC Converter</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Direct conversion dc-dc converter serves data centers</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Electronic Products &amp; Technology</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>https://www.ept.ca/products/direct-conversion-dc-dc-converter-serves-data-centers/</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>DC-DC Converter DCDC</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>High-voltage DC-DC converters for power electronics in noise-sensitive applications introduced by TDK Lambda</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Military &amp; Aerospace Electronics</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://www.militaryaerospace.com/power/article/14205250/dcdc-converters-power-highvoltage</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>BMS</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>BMS' Opdivo/relatlimab combination gets boost in LoA in 1L melanoma</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Clinical Trials Arena</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://www.clinicaltrialsarena.com/comment/loa-update-bms-opdivo-relatlimab-combination-gets-boost-in-approval-likelihood-after-phase-ii-iii-results/</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>BMS</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>CCNJ CONGRATULATES MEMBERS BRISTOL MYERS SQUIBB AND MERCK &amp; CO., RECIPIENTS OF THE 2021 EPA GREEN CHEMISTRY CHALLENGE AWARD</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>InsiderNJ</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://www.insidernj.com/press-release/ccnj-congratulates-members-bristol-myers-squibb-merck-co-recipients-2021-epa-green-chemistry-challenge-award/</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>BMS Cloud</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>PRNewswire</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Industry</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>BMS Cloud</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>EcoXpert Awards: AZZO wins “Project of the Year”</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Marketscreener.com</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://www.marketscreener.com/quote/stock/SCHNEIDER-ELECTRIC-SE-4699/news/EcoXpert-Awards-AZZO-wins-ldquo-Project-of-the-Year-rdquo-35624009/</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Energy Management Unit</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Installation cost of energy management system is very high which is considered to be a major restraint for the market – KSU | The Sentinel Newspaper</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>KSU | The Sentinel Newspaper</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://ksusentinel.com/2021/06/15/installation-cost-of-energy-management-system-is-very-high-which-is-considered-to-be-a-major-restraint-for-the-market/</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>06/15/2021</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Placeholder</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Product</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Energy Management Unit</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Latest Update 2021: Global Building Energy Management System (BEMS) Market by COVID-19 Impact Analysis by Market Research Store – KSU | The Sentinel Newspaper</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>KSU | The Sentinel Newspaper</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://ksusentinel.com/2021/06/16/latest-update-2021-global-building-energy-management-system-bems-market-by-covid-19-impact-analysis-by-market-research-store/</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>06/16/2021</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
         <is>
           <t>Placeholder</t>
         </is>

</xml_diff>

<commit_message>
Added basic error handling when accessing the article site using the Requests library
</commit_message>
<xml_diff>
--- a/CatchAll.xlsx
+++ b/CatchAll.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H39"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -486,7 +486,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>EV Relay Market Size, Industry Trends and Forecast to 2028 | Major Players – Panasonic, TE Connectivity, Omron, HELLA, Fujitsu, LSIS – The Courier</t>
+          <t>Keyless Vehicle Access Control Systems Market 2021 Opportunities and Key Players to 2026 – Denso, ZF, Hella. – The Courier</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -496,12 +496,12 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://www.mccourier.com/ev-relay-market-size-industry-trends-and-forecast-to-2028-major-players-panasonic-te-connectivity-omron-hella-fujitsu-lsis/</t>
+          <t>https://www.mccourier.com/keyless-vehicle-access-control-systems-market-2021-opportunities-and-key-players-to-2026-denso-zf-hella/</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
@@ -526,22 +526,22 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Global Vehicle Security Market demand 2021 | Continental, Delphi Automotive, Hella KGaA Hueck, Tokai Rika – KSU | The Sentinel Newspaper</t>
+          <t>Side Turn Signal Lamp Market Competitive Analysis, Demand, Business Outlook and Forecasts 2027| Hella, Stanley, Truck-Lite, Wenzhou Bosheng Automotive Parts, Sunlight, Bosch, Koito – The Manomet Current</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>KSU | The Sentinel Newspaper</t>
+          <t>The Manomet Current</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://ksusentinel.com/2021/06/16/global-vehicle-security-market-demand-2021-continental-delphi-automotive-hella-kgaa-hueck-tokai-rika/</t>
+          <t>https://manometcurrent.com/side-turn-signal-lamp-market-competitive-analysis-demand-business-outlook-and-forecasts-2027-hella-stanley-truck-lite-wenzhou-bosheng-automotive-parts-sunlight-bosch-koito/</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -566,22 +566,22 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Key Foundry Offers ABOV Semiconductor Gen2 Flash Memory Embedded 0.13 micron BCD Process Suitable for Automotive Power Semiconductor</t>
+          <t>Automotive Power Liftgate Market to Grow on an Exceptional Note in the Next Few Years: Huf, Brose, Magna, HI-LEX – The Manomet Current</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>PRNewswire</t>
+          <t>The Manomet Current</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://www.prnewswire.com/news-releases/key-foundry-offers-abov-semiconductor-gen2-flash-memory-embedded-0-13-micron-bcd-process-suitable-for-automotive-power-semiconductor-301312052.html</t>
+          <t>https://manometcurrent.com/automotive-power-liftgate-market-to-grow-on-an-exceptional-note-in-the-next-few-years-huf-brose-magna-hi-lex/</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
@@ -606,7 +606,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Automotive Power Distribution Modules Market Size, Trends, Growth, Scope, Overall Analysis and Forecast by 2028 – The Manomet Current</t>
+          <t>Global Automotive Power Modules Market 2020 Analysis, Future Industry, Growth Rate, Key Players and Forecast to 2025 – The Manomet Current</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -616,12 +616,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/automotive-power-distribution-modules-market-size-trends-growth-scope-overall-analysis-and-forecast-by-2028/</t>
+          <t>https://manometcurrent.com/global-automotive-power-modules-market-2020-analysis-future-industry-growth-rate-key-players-and-forecast-to-2025/</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -646,22 +646,22 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
+          <t>US energy secretary: 'We need to act now to develop domestic lithium battery capabilities'</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>Energy Storage News</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
+          <t>https://www.energy-storage.news/blogs/us-energy-secretary-we-need-to-act-now-to-develop-domestic-lithium-battery</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
@@ -686,22 +686,22 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Environment + Energy Leader</t>
+          <t>The Manomet Current</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
@@ -726,22 +726,22 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Environment + Energy Leader</t>
+          <t>The Manomet Current</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -766,22 +766,22 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
+          <t>US energy secretary: 'We need to act now to develop domestic lithium battery capabilities'</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>Energy Storage News</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
+          <t>https://www.energy-storage.news/blogs/us-energy-secretary-we-need-to-act-now-to-develop-domestic-lithium-battery</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
@@ -806,22 +806,22 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Environment + Energy Leader</t>
+          <t>The Manomet Current</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
@@ -846,22 +846,22 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Battery Management System Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – Storage Battery Systems, Eberspaecher Vecture, Leclanche, Nuvation Engineering, Lithium Balance, Johnson Matthey – The Manomet Curr</t>
+          <t>US energy secretary: 'We need to act now to develop domestic lithium battery capabilities'</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>Energy Storage News</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/battery-management-system-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-storage-battery-systems-eberspaecher-vecture-leclanche-nuvation-engineering-lithium-ba/</t>
+          <t>https://www.energy-storage.news/blogs/us-energy-secretary-we-need-to-act-now-to-develop-domestic-lithium-battery</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
@@ -886,22 +886,22 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Manual Disconnect Switch Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – ABB, Sensata Technologies, Omega Engineering, Schneider Electric, Walther-Werke, TTI – The Manomet Current</t>
+          <t>Global Temperature Monitoring Market Innovative Strategy by 2028, Industry Growth | Emerson, Sensata, Amphenol, TE Connectivity, Texas instruments Inc., Molex, Honeywell – KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/manual-disconnect-switch-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-abb-sensata-technologies-omega-engineering-schneider-electric-walther-werke-tti/</t>
+          <t>https://ksusentinel.com/2021/06/17/global-temperature-monitoring-market-innovative-strategy-by-2028-industry-growth-emerson-sensata-amphenol-te-connectivity-texas-instruments-inc-molex-honeywell/</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
@@ -926,22 +926,22 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Electromechanical Pressure Switch Market Size and Growth Opportunities with COVID19 Impact Analysis | Top Companies – GTE Elettromeccanica, ENERPAC, Norgren, IMI Precision Engineering, Sensata Technologies, Barksdale – The Manomet Current</t>
+          <t>Global Exhaust Sensors Market 2021-2028 Value, Region, Trends Sensata Technologies, ABB, Analog Devices – The Courier</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>The Courier</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/electromechanical-pressure-switch-market-size-and-growth-opportunities-with-covid19-impact-analysis-top-companies-gte-elettromeccanica-enerpac-norgren-imi-precision-engineering-sensata-technol/</t>
+          <t>https://www.mccourier.com/global-exhaust-sensors-market-2021-2028-value-region-trends-sensata-technologies-abb-analog-devices/</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/15/2021</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
@@ -966,22 +966,22 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Automotive Pressure Sensors Market 2021: Analysis by Business Development, Concentration Rate| Infineon Technologies AG, Sensata Technologies Inc, Texas Instruments Incorporated – The Manomet Current</t>
+          <t>Ossia Announces CotaReal Wireless Power Trailer Tracker System</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>Illinoisnewstoday.com</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/automotive-pressure-sensors-market-2021-analysis-by-business-development-concentration-rate-infineon-technologies-ag-sensata-technologies-inc-texas-instruments-incorporated/</t>
+          <t>https://illinoisnewstoday.com/ossia-announces-cotareal-wireless-power-trailer-tracker-system/254627/</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>06/14/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
@@ -992,36 +992,36 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Competitor</t>
+          <t>Customer</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Sensata Battery Management System</t>
+          <t>Lordstown</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Global Automotive MEMS Sensors Market 2021: Segmentation Application, Technology &amp; Market Analysis Research Report to 2024 – Out 'n Proud</t>
+          <t>Lordstown Motors: No binding offers yet for electric Endurance pickup truck</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Out 'n Proud</t>
+          <t>Massillon Independent</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://onpblog.com/uncategorized/30573/global-automotive-mems-sensors-market-2021-segmentation-application-technology-market-analysis-research-report-to-2024/</t>
+          <t>https://www.indeonline.com/story/news/2021/06/17/lordstown-motors-says-no-binding-offers-new-electric-pickup-truck/7732165002/</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1032,7 +1032,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1046,17 +1046,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Company with ties to Lordstown Motors to challenge USPS contract decision</t>
+          <t>Lordstown Motors execs cite binding orders to restore confidence a day after CEO, CFO resignations</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>WFMJ</t>
+          <t>TechCrunch</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://www.wfmj.com/story/44116835/company-with-ties-to-lordstown-motors-to-challenge-usps-contract-decision</t>
+          <t>https://techcrunch.com/2021/06/15/lordstown-motors-execs-cite-binding-orders-to-restore-confidence-a-day-after-ceo-cfo-resignations/</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1072,36 +1072,36 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Customer</t>
+          <t>Industry</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Lordstown</t>
+          <t>Battery Management System</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>Lordstown's Struggles Raise New Fears About SPACs</t>
+          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>The New York Times</t>
+          <t>PRNewswire</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://www.nytimes.com/2021/06/15/business/dealbook/lordstown-spacs-sec.html</t>
+          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
@@ -1112,7 +1112,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1126,22 +1126,22 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Battery Management Systems Market to Leap 15% per Year through 2030</t>
+          <t>Aircraft Battery Management System (BMS) Market Emerging Trends, Size, Share, Regional Outlook by 2028 | Concorde Battery, MarathonNorco Aerospace, Saft, Acme Aerospace, EaglePicher Technologies, Kanto Aircraft Instrument – KSU | The Sentinel Ne</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Environment + Energy Leader</t>
+          <t>KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://www.environmentalleader.com/2021/06/198420/</t>
+          <t>https://ksusentinel.com/2021/06/17/aircraft-battery-management-system-bms-market-emerging-trends-size-share-regional-outlook-by-2028-concorde-battery-marathonnorco-aerospace-saft-acme-aerospace-eaglepicher-technologies/</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
@@ -1152,7 +1152,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1161,27 +1161,27 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Battery Management System</t>
+          <t>Battery Management System Cloud</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Electric Vehicle Battery Management System Market Trends 2021 Share, Growth Factor, Industry Size, Major Key Players, Type and Analysis with Covid-19 Impact till 2027 – The Manomet Current</t>
+          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>The Manomet Current</t>
+          <t>PRNewswire</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://manometcurrent.com/electric-vehicle-battery-management-system-market-trends-2021-share-growth-factor-industry-size-major-key-players-type-and-analysis-with-covid-19-impact-till-2027/</t>
+          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
@@ -1192,7 +1192,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1206,17 +1206,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
+          <t>Lincoln to introduce four new battery-electric vehicles starting next year</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>PRNewswire</t>
+          <t>The Detroit News</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
+          <t>https://www.detroitnews.com/story/business/autos/ford/2021/06/16/lincoln-introduce-four-new-battery-electric-vehicles-starting-next-year/7693304002/</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1232,7 +1232,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1241,27 +1241,27 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Battery Management System Cloud</t>
+          <t>Battery Management System BMS</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Lincoln to introduce four new battery-electric vehicles starting next year</t>
+          <t>Aircraft Battery Management System (BMS) Market Emerging Trends, Size, Share, Regional Outlook by 2028 | Concorde Battery, MarathonNorco Aerospace, Saft, Acme Aerospace, EaglePicher Technologies, Kanto Aircraft Instrument – KSU | The Sentinel Ne</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>The Detroit News</t>
+          <t>KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://www.detroitnews.com/story/business/autos/ford/2021/06/16/lincoln-introduce-four-new-battery-electric-vehicles-starting-next-year/7693304002/</t>
+          <t>https://ksusentinel.com/2021/06/17/aircraft-battery-management-system-bms-market-emerging-trends-size-share-regional-outlook-by-2028-concorde-battery-marathonnorco-aerospace-saft-acme-aerospace-eaglepicher-technologies/</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1272,7 +1272,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1286,17 +1286,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
+          <t>Global Energy storage (ES) battery management system (BMS) Market 2021 Consumer Needs – Nuvation Energy, Leclanché, Ion Energy Inc, Sunceco – The Courier</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>PRNewswire</t>
+          <t>The Courier</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
+          <t>https://www.mccourier.com/global-energy-storage-es-battery-management-system-bms-market-2021-consumer-needs-nuvation-energy-leclanche-ion-energy-inc-sunceco/</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1312,7 +1312,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1321,27 +1321,27 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Battery Management System BMS</t>
+          <t>CCS</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Leclanché introduces new generation of Li-ion modules for e-transport; high-volume production line</t>
+          <t>CCS baseball, track and field championship weekend: What to know</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Green Car Congress</t>
+          <t>The Mercury News</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://www.greencarcongress.com/2021/06/20210616-leclanche.html</t>
+          <t>https://www.mercurynews.com/2021/06/17/ccs-baseball-track-and-field-championship-weekend-what-to-know/</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -1352,7 +1352,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1366,22 +1366,22 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>Christopher’s Fantastic Four headed to CCS Track and Field Finals</t>
+          <t>CCS baseball roundup: Sequoia, Los Altos, Burlingame advance to championship games</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Gilroy Dispatch</t>
+          <t>The Mercury News</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://gilroydispatch.com/christophers-fantastic-four-headed-to-ccs-track-and-field-finals/</t>
+          <t>https://www.mercurynews.com/2021/06/17/ccs-baseball-roundup-sequoia-los-altos-burlingame-advance-to-championship-games/</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
@@ -1392,7 +1392,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1401,27 +1401,27 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>CCS</t>
+          <t>Electric Vehicle Charge Controller</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>San Juan coal plant stays open for CCS conversion</t>
+          <t>The 7 Best Startups You Can Buy on StartEngine Right Now</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Power Engineering International</t>
+          <t>InvestorPlace</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://www.powerengineeringint.com/coal-fired/san-juan-coal-plant-stays-open-for-ccs-conversion/</t>
+          <t>https://investorplace.com/2021/06/the-7-best-startups-you-can-buy-on-startengine-right-now-4/</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
@@ -1432,7 +1432,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1446,17 +1446,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Delta-Q Technologies Launches the new XV3300 Battery Charging Solution</t>
+          <t>Skodatown: behind the scenes at Skoda's Czech factory</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Rental Equipment Register</t>
+          <t>AutoExpress</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://www.rermag.com/directory/automotive-tools-equipment/batteries/article/21167043/deltaq-technologies-launches-the-new-xv3300-battery-charging-solution</t>
+          <t>https://www.autoexpress.co.uk/skoda/enyaq/109116/skoda-enyaq-iv-sale-now-ps31085/production</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1472,7 +1472,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1481,27 +1481,27 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Electric Vehicle Charge Controller</t>
+          <t>Fast Charge Junction Box</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Everything we know about the Huawei Seres SF5 SUV</t>
+          <t>City schools name teacher of the year</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Illinoisnewstoday.com</t>
+          <t>Mount Airy News</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://illinoisnewstoday.com/everything-we-know-about-the-huawei-seres-sf5-suv/249924/</t>
+          <t>https://www.mtairynews.com/news/98467/city-schools-name-teacher-of-the-year</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>06/14/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
@@ -1512,7 +1512,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1521,27 +1521,27 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Electric Vehicle Charge Controller EVCC</t>
+          <t>Fast Charge Junction Box</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Electric Vehicle Communication Controllers market 2021-2028: ABB Ltd. BYD Co Ltd. ENGIE Ficosa International SA LG INNOTEK Mitsubishi Electric Corporation Robert Bosch GmbH Schneider Electric SE Siemens AG Tesla, Inc. – Miner News</t>
+          <t>Ruritans look to help Spark of Hope</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Miner News</t>
+          <t>Mount Airy News</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://minernews.io/space/193144/electric-vehicle-communication-controllers-market-2021-2028-abb-ltd-byd-co-ltd-engie-ficosa-international-s-a-lg-innotek-mitsubishi-electric-corporation-robert-2/</t>
+          <t>https://www.mtairynews.com/news/98453/ruritans-look-to-help-spark-of-hope</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
@@ -1561,27 +1561,27 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Fast Charge Junction Box</t>
+          <t>DC-DC Converter</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>County to kick-off 250th celebration</t>
+          <t>High-voltage DC-DC converters for power electronics in noise-sensitive applications introduced by TDK Lambda</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Mount Airy News</t>
+          <t>Intelligent Aerospace</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://www.mtairynews.com/news/98435/county-to-kick-off-250th-celebration</t>
+          <t>https://www.intelligent-aerospace.com/military/article/14205375/highvoltage-dcdc-converters-for-power-electronics-in-noisesensitive-applications-introduced-by-tdk-lambda</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
@@ -1601,27 +1601,27 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Fast Charge Junction Box</t>
+          <t>DC-DC Converter</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Open House offers glimpse to the past</t>
+          <t>ROHM Introduces Industry-first AC/DC Converter ICs in a Surface Mount Package with Built-in</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Mount Airy News</t>
+          <t>GlobeNewswire</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://www.mtairynews.com/news/98431/open-house-offers-glimpse-to-the-past</t>
+          <t>https://www.globenewswire.com/news-release/2021/06/17/2249350/0/en/ROHM-Introduces-Industry-first-AC-DC-Converter-ICs-in-a-Surface-Mount-Package-with-Built-in-1700V-SiC-MOSFET.html</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
@@ -1641,7 +1641,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>DC-DC Converter</t>
+          <t>DC-DC Converter DCDC</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1651,17 +1651,17 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Military &amp; Aerospace Electronics</t>
+          <t>Intelligent Aerospace</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>https://www.militaryaerospace.com/power/article/14205250/dcdc-converters-power-highvoltage</t>
+          <t>https://www.intelligent-aerospace.com/military/article/14205375/highvoltage-dcdc-converters-for-power-electronics-in-noisesensitive-applications-introduced-by-tdk-lambda</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
@@ -1672,7 +1672,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -1681,22 +1681,22 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>DC-DC Converter</t>
+          <t>BMS</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Direct conversion dc-dc converter serves data centers</t>
+          <t>BMS' Opdivo/relatlimab combination gets boost in LoA in 1L melanoma</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Electronic Products &amp; Technology</t>
+          <t>Clinical Trials Arena</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>https://www.ept.ca/products/direct-conversion-dc-dc-converter-serves-data-centers/</t>
+          <t>https://www.clinicaltrialsarena.com/comment/loa-update-bms-opdivo-relatlimab-combination-gets-boost-in-approval-likelihood-after-phase-ii-iii-results/</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1712,7 +1712,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -1721,27 +1721,27 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>DC-DC Converter DCDC</t>
+          <t>BMS</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>High-voltage DC-DC converters for power electronics in noise-sensitive applications introduced by TDK Lambda</t>
+          <t>BMS Vidarbha Pradesh elects new team</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Military &amp; Aerospace Electronics</t>
+          <t>The Hitavada</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>https://www.militaryaerospace.com/power/article/14205250/dcdc-converters-power-highvoltage</t>
+          <t>https://www.thehitavada.com/Encyc/2021/6/17/BMS-Vidarbha-Pradesh-elects-new-team.html</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>06/15/2021</t>
+          <t>06/16/2021</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
@@ -1761,22 +1761,22 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>BMS</t>
+          <t>BMS Cloud</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>BMS' Opdivo/relatlimab combination gets boost in LoA in 1L melanoma</t>
+          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Clinical Trials Arena</t>
+          <t>PRNewswire</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>https://www.clinicaltrialsarena.com/comment/loa-update-bms-opdivo-relatlimab-combination-gets-boost-in-approval-likelihood-after-phase-ii-iii-results/</t>
+          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1801,27 +1801,27 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>BMS</t>
+          <t>BMS Cloud</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>CCNJ CONGRATULATES MEMBERS BRISTOL MYERS SQUIBB AND MERCK &amp; CO., RECIPIENTS OF THE 2021 EPA GREEN CHEMISTRY CHALLENGE AWARD</t>
+          <t>Cost watchdog ICER will bless some high-priced gene and cell therapies, but only with solid proof of benefit: Analyst</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>InsiderNJ</t>
+          <t>FiercePharma</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>https://www.insidernj.com/press-release/ccnj-congratulates-members-bristol-myers-squibb-merck-co-recipients-2021-epa-green-chemistry-challenge-award/</t>
+          <t>https://www.fiercepharma.com/pharma/cost-watchdog-icer-will-bless-some-high-priced-gene-and-cell-therapies-but-only-solid-proof</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
@@ -1836,32 +1836,32 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Industry</t>
+          <t>Product</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>BMS Cloud</t>
+          <t>Energy Management Unit</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Global Battery Management System Market Report 2021: Market Value is Projected to Grow from $5,661.0 Million in 2020 to $22,279.6 Million by 2030, at a 15.0% CAGR</t>
+          <t>What is the ongoing demand scene for Energy Management System Market? in the European and Australian – KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>PRNewswire</t>
+          <t>KSU | The Sentinel Newspaper</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>https://www.prnewswire.com/news-releases/global-battery-management-system-market-report-2021-market-value-is-projected-to-grow-from-5-661-0-million-in-2020-to-22-279-6-million-by-2030--at-a-15-0-cagr-301313614.html</t>
+          <t>https://ksusentinel.com/2021/06/17/what-is-the-ongoing-demand-scene-for-energy-management-system-market-in-the-european-and-australian/</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
@@ -1876,115 +1876,35 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Industry</t>
+          <t>Product</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>BMS Cloud</t>
+          <t>Energy Management Unit</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>EcoXpert Awards: AZZO wins “Project of the Year”</t>
+          <t>Ford™ Acquires Electriphi to Provide Ford Pro Commercial Customers with Seamless Charging and Energy Management</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Marketscreener.com</t>
+          <t>Business Wire</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>https://www.marketscreener.com/quote/stock/SCHNEIDER-ELECTRIC-SE-4699/news/EcoXpert-Awards-AZZO-wins-ldquo-Project-of-the-Year-rdquo-35624009/</t>
+          <t>https://www.businesswire.com/news/home/20210617005640/en/Ford%E2%84%A2-Acquires-Electriphi-to-Provide-Ford-Pro-Commercial-Customers-with-Seamless-Charging-and-Energy-Management</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>06/16/2021</t>
+          <t>06/17/2021</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
-        <is>
-          <t>Placeholder</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>Energy Management Unit</t>
-        </is>
-      </c>
-      <c r="D38" t="inlineStr">
-        <is>
-          <t>Installation cost of energy management system is very high which is considered to be a major restraint for the market – KSU | The Sentinel Newspaper</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>KSU | The Sentinel Newspaper</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>https://ksusentinel.com/2021/06/15/installation-cost-of-energy-management-system-is-very-high-which-is-considered-to-be-a-major-restraint-for-the-market/</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>06/15/2021</t>
-        </is>
-      </c>
-      <c r="H38" t="inlineStr">
-        <is>
-          <t>Placeholder</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Product</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Energy Management Unit</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Latest Update 2021: Global Building Energy Management System (BEMS) Market by COVID-19 Impact Analysis by Market Research Store – KSU | The Sentinel Newspaper</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>KSU | The Sentinel Newspaper</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>https://ksusentinel.com/2021/06/16/latest-update-2021-global-building-energy-management-system-bems-market-by-covid-19-impact-analysis-by-market-research-store/</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>06/16/2021</t>
-        </is>
-      </c>
-      <c r="H39" t="inlineStr">
         <is>
           <t>Placeholder</t>
         </is>

</xml_diff>